<commit_message>
changed template to Excel spreadsheet and adjusted app as needed
</commit_message>
<xml_diff>
--- a/data/example_data/one_obs_extra_vars.xlsx
+++ b/data/example_data/one_obs_extra_vars.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinegoode/Desktop/carp-rf/shiny-app/app/data/example_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C436857F-9555-CF47-BC04-D38D302E2E2D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F73F82FE-8951-4A47-8F87-DE77C0BDDA0C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440" xr2:uid="{A53B36F3-758C-E94F-81F2-A98347AF26C7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{A53B36F3-758C-E94F-81F2-A98347AF26C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>Dataset</t>
   </si>
@@ -99,21 +99,6 @@
     <t>Deflated</t>
   </si>
   <si>
-    <t>Genus</t>
-  </si>
-  <si>
-    <t>Common_Name</t>
-  </si>
-  <si>
-    <t>Family_ACGC</t>
-  </si>
-  <si>
-    <t>Genus_ACGC</t>
-  </si>
-  <si>
-    <t>Common_Name_ACGC</t>
-  </si>
-  <si>
     <t>original</t>
   </si>
   <si>
@@ -132,22 +117,10 @@
     <t>N</t>
   </si>
   <si>
-    <t>Aplodinotus</t>
-  </si>
-  <si>
-    <t>Freshwater Drum</t>
-  </si>
-  <si>
-    <t>Sciaenidae</t>
-  </si>
-  <si>
     <t>Egg_ID</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>2014-07-27</t>
+    <t>Day</t>
   </si>
 </sst>
 </file>
@@ -183,9 +156,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,17 +472,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60505E87-C4CA-C046-88BD-309199189A78}">
-  <dimension ref="A1:AB2"/>
+  <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -522,13 +492,13 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
@@ -578,43 +548,28 @@
       <c r="W1" t="s">
         <v>20</v>
       </c>
-      <c r="X1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>25</v>
-      </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2">
+        <v>2014</v>
+      </c>
+      <c r="F2">
+        <v>7</v>
+      </c>
+      <c r="G2">
         <v>27</v>
-      </c>
-      <c r="D2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2">
-        <v>2014</v>
-      </c>
-      <c r="G2">
-        <v>7</v>
       </c>
       <c r="H2">
         <v>209</v>
@@ -650,34 +605,19 @@
         <v>3.0539479000000001E-2</v>
       </c>
       <c r="S2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="T2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="U2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="V2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="W2" t="s">
-        <v>31</v>
-      </c>
-      <c r="X2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>